<commit_message>
v1.2.99.90: minor parameter changes + lexion 670
</commit_message>
<xml_diff>
--- a/Documents/AdvancedClutchParameters.xlsx
+++ b/Documents/AdvancedClutchParameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="0" windowWidth="22965" windowHeight="13020"/>
+    <workbookView xWindow="3120" yWindow="0" windowWidth="22965" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -502,34 +502,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.90625E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.2592592592592622E-3</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.407407407407407E-2</c:v>
+                  <c:v>0.10546874999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25000000000000017</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59259259259259278</c:v>
+                  <c:v>0.48828125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1574074074074077</c:v>
+                  <c:v>0.84374999999999956</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>1.3398437499999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.1759259259259269</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.7407407407407423</c:v>
+                  <c:v>2.84765625</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.75</c:v>
+                  <c:v>3.90625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,11 +544,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="360796792"/>
-        <c:axId val="360795224"/>
+        <c:axId val="316048864"/>
+        <c:axId val="316048080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="360796792"/>
+        <c:axId val="316048864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -606,12 +606,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360795224"/>
+        <c:crossAx val="316048080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="360795224"/>
+        <c:axId val="316048080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -669,7 +669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="360796792"/>
+        <c:crossAx val="316048864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1350,10 +1350,10 @@
     <tableColumn id="3" name="clutchTo"/>
     <tableColumn id="4" name="clutchExp"/>
     <tableColumn id="5" name="clutchFactor"/>
-    <tableColumn id="6" name="0" dataDxfId="0">
+    <tableColumn id="6" name="0" dataDxfId="1">
       <calculatedColumnFormula>IF(F$1&lt;$B2,0,IF(F$1&gt;$C2,$E2,$E2*((F$1-$B2)/($C2-$B2))^$D2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="0.1" dataDxfId="1">
+    <tableColumn id="7" name="0.1" dataDxfId="0">
       <calculatedColumnFormula>IF(G$1&lt;Table1[[#This Row],[clutchFrom]],0,IF(G$1&gt;Table1[[#This Row],[clutchExp]],Table1[[#This Row],[0]],Table1[[#This Row],[0]]*((G$1-Table1[[#This Row],[clutchTo]])/(Table1[[#This Row],[clutchExp]]-Table1[[#This Row],[clutchTo]]))^Table1[[#This Row],[clutchFactor]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" name="0.2">
@@ -1654,7 +1654,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,10 +1892,10 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -1909,43 +1909,43 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.90625E-3</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>9.2592592592592622E-3</v>
+        <v>3.125E-2</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>7.407407407407407E-2</v>
+        <v>0.10546874999999994</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0.25000000000000017</v>
+        <v>0.25</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>0.59259259259259278</v>
+        <v>0.48828125</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>1.1574074074074077</v>
+        <v>0.84374999999999956</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.3398437499999993</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>3.1759259259259269</v>
+        <v>2</v>
       </c>
       <c r="O5">
         <f t="shared" si="1"/>
-        <v>4.7407407407407423</v>
+        <v>2.84765625</v>
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
-        <v>6.75</v>
+        <v>3.90625</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.2.99.93: smoother clutch if clutchOpenRpm > idleRpm
</commit_message>
<xml_diff>
--- a/Documents/AdvancedClutchParameters.xlsx
+++ b/Documents/AdvancedClutchParameters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="0" windowWidth="22965" windowHeight="13020"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="22965" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,34 +389,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8309037900874661E-3</c:v>
+                  <c:v>3.90625E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6647230320699729E-2</c:v>
+                  <c:v>3.125E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15743440233236156</c:v>
+                  <c:v>0.10546874999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.37317784256559783</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.72886297376093301</c:v>
+                  <c:v>0.48828125</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2594752186588924</c:v>
+                  <c:v>0.84374999999999956</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>1.3398437499999993</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>2.9854227405247826</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.2507288629737623</c:v>
+                  <c:v>2.84765625</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.8309037900874641</c:v>
+                  <c:v>3.90625</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -502,34 +502,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.90625E-3</c:v>
+                  <c:v>2.4740773326991775E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>0.11367874248827986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.10546874999999994</c:v>
+                  <c:v>0.27738312123103165</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25</c:v>
+                  <c:v>0.52233033797767447</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.48828125</c:v>
+                  <c:v>0.85338947016847511</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.84374999999999956</c:v>
+                  <c:v>1.2745181402481172</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3398437499999993</c:v>
+                  <c:v>1.7890766943803709</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>2.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.84765625</c:v>
+                  <c:v>3.1099026262015643</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.90625</c:v>
+                  <c:v>3.9211483222172747</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -544,11 +544,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="316048864"/>
-        <c:axId val="316048080"/>
+        <c:axId val="340400120"/>
+        <c:axId val="340395416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="316048864"/>
+        <c:axId val="340400120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -606,12 +606,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316048080"/>
+        <c:crossAx val="340395416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="316048080"/>
+        <c:axId val="340395416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5"/>
@@ -669,7 +669,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="316048864"/>
+        <c:crossAx val="340400120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1654,7 +1654,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1834,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -1848,43 +1848,43 @@
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>5.8309037900874661E-3</v>
+        <v>3.90625E-3</v>
       </c>
       <c r="H4">
         <f t="shared" si="0"/>
-        <v>4.6647230320699729E-2</v>
+        <v>3.125E-2</v>
       </c>
       <c r="I4">
         <f t="shared" si="0"/>
-        <v>0.15743440233236156</v>
+        <v>0.10546874999999994</v>
       </c>
       <c r="J4">
         <f t="shared" si="0"/>
-        <v>0.37317784256559783</v>
+        <v>0.25</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>0.72886297376093301</v>
+        <v>0.48828125</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>1.2594752186588924</v>
+        <v>0.84374999999999956</v>
       </c>
       <c r="M4">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1.3398437499999993</v>
       </c>
       <c r="N4">
         <f t="shared" si="1"/>
-        <v>2.9854227405247826</v>
+        <v>2</v>
       </c>
       <c r="O4">
         <f t="shared" si="1"/>
-        <v>4.2507288629737623</v>
+        <v>2.84765625</v>
       </c>
       <c r="P4">
         <f t="shared" si="1"/>
-        <v>5.8309037900874641</v>
+        <v>3.90625</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1898,10 +1898,10 @@
         <v>0.8</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
@@ -1909,43 +1909,43 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>3.90625E-3</v>
+        <v>2.4740773326991775E-2</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>3.125E-2</v>
+        <v>0.11367874248827986</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>0.10546874999999994</v>
+        <v>0.27738312123103165</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>0.25</v>
+        <v>0.52233033797767447</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>0.48828125</v>
+        <v>0.85338947016847511</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>0.84374999999999956</v>
+        <v>1.2745181402481172</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>1.3398437499999993</v>
+        <v>1.7890766943803709</v>
       </c>
       <c r="N5">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.4</v>
       </c>
       <c r="O5">
         <f t="shared" si="1"/>
-        <v>2.84765625</v>
+        <v>3.1099026262015643</v>
       </c>
       <c r="P5">
         <f t="shared" si="1"/>
-        <v>3.90625</v>
+        <v>3.9211483222172747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>